<commit_message>
att 2 desenvolvimento do proj
</commit_message>
<xml_diff>
--- a/Sprint 2/Entregáveis 2/Planilha de riscos 1.xlsx
+++ b/Sprint 2/Entregáveis 2/Planilha de riscos 1.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jotin\Desktop\Bolt Tech\Bolt-Tech\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Joao Pedro (Black)\Faculade\PROJETO BOLTTECH\Bolt-Tech\Sprint 2\Entregáveis 2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D086E09-C197-4586-B084-5E6C354121A7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0063D550-B9E0-48FB-A4F6-43555CB7F5DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{9F098431-5A62-43C5-8B6D-4B634E5E6ADC}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
   <si>
     <t>Probalidade/Impacto</t>
   </si>
@@ -81,9 +81,6 @@
     <t>Grave (9)</t>
   </si>
   <si>
-    <t>Gravíssimo (10)</t>
-  </si>
-  <si>
     <t>Impacto</t>
   </si>
   <si>
@@ -94,13 +91,37 @@
   </si>
   <si>
     <t>Integrante se recusar a colaborar com a equipe</t>
+  </si>
+  <si>
+    <t>Plano de resposta</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reorganização de tarefas entre os remanescentes </t>
+  </si>
+  <si>
+    <t>Explicar novamente o motivo da dúvida</t>
+  </si>
+  <si>
+    <t>Revisão do Código</t>
+  </si>
+  <si>
+    <t>Aumentar comunicação entre os integrantes</t>
+  </si>
+  <si>
+    <t>Conversar com superiores para ajudar a resolver</t>
+  </si>
+  <si>
+    <t>Cobrança maior sobre o atraso e cuidado para a não reincidencia</t>
+  </si>
+  <si>
+    <t>Muito Grave (10)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -111,6 +132,14 @@
     <font>
       <b/>
       <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -149,7 +178,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="17">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -186,19 +215,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="medium">
         <color indexed="64"/>
       </left>
@@ -238,8 +254,34 @@
       <right style="medium">
         <color indexed="64"/>
       </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
       <top/>
-      <bottom style="thin">
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -249,136 +291,32 @@
       <right style="medium">
         <color indexed="64"/>
       </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
       <top/>
       <bottom style="medium">
         <color indexed="64"/>
       </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thick">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thick">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thick">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thick">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -391,63 +329,51 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -764,18 +690,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5228A790-DC29-4987-96DE-D54C6D496301}">
   <dimension ref="A1:F21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="18.81640625" customWidth="1"/>
-    <col min="2" max="2" width="14.453125" customWidth="1"/>
-    <col min="3" max="3" width="40.54296875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.54296875" customWidth="1"/>
+    <col min="2" max="2" width="42.26953125" customWidth="1"/>
+    <col min="3" max="3" width="27.36328125" customWidth="1"/>
     <col min="4" max="4" width="34.1796875" customWidth="1"/>
-    <col min="5" max="5" width="33.81640625" customWidth="1"/>
-    <col min="6" max="6" width="13.81640625" customWidth="1"/>
+    <col min="5" max="5" width="55.36328125" customWidth="1"/>
+    <col min="6" max="6" width="42.26953125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
@@ -796,7 +722,7 @@
         <v>14</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>15</v>
+        <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -904,91 +830,104 @@
       <c r="B9" s="1"/>
     </row>
     <row r="10" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C10" s="22" t="s">
+      <c r="B10" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="D10" s="21" t="s">
+      <c r="C10" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="E10" s="33" t="s">
+      <c r="D10" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="E10" s="21" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B11" s="22" t="s">
+        <v>9</v>
+      </c>
+      <c r="C11" s="22">
+        <v>10</v>
+      </c>
+      <c r="D11" s="23"/>
+      <c r="E11" s="27" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B12" s="22" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="C11" s="20" t="s">
+      <c r="C12" s="22">
+        <v>12</v>
+      </c>
+      <c r="D12" s="24"/>
+      <c r="E12" s="25" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B13" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="D11" s="19">
+      <c r="C13" s="22">
         <v>18</v>
       </c>
-      <c r="E11" s="27"/>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="C12" s="23" t="s">
-        <v>9</v>
-      </c>
-      <c r="D12" s="24">
+      <c r="D13" s="26"/>
+      <c r="E13" s="27" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B14" s="22" t="s">
+        <v>17</v>
+      </c>
+      <c r="C14" s="22">
+        <v>21</v>
+      </c>
+      <c r="D14" s="28"/>
+      <c r="E14" s="27" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B15" s="22" t="s">
+        <v>18</v>
+      </c>
+      <c r="C15" s="22">
+        <v>20</v>
+      </c>
+      <c r="D15" s="29"/>
+      <c r="E15" s="27" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B16" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="E12" s="28"/>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="C13" s="23" t="s">
-        <v>10</v>
-      </c>
-      <c r="D13" s="24">
+      <c r="C16" s="22">
         <v>27</v>
       </c>
-      <c r="E13" s="29"/>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="C14" s="23" t="s">
-        <v>17</v>
-      </c>
-      <c r="D14" s="24">
-        <v>12</v>
-      </c>
-      <c r="E14" s="30"/>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="C15" s="23" t="s">
-        <v>18</v>
-      </c>
-      <c r="D15" s="24">
-        <v>21</v>
-      </c>
-      <c r="E15" s="31"/>
-    </row>
-    <row r="16" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C16" s="25" t="s">
-        <v>19</v>
-      </c>
-      <c r="D16" s="26">
-        <v>20</v>
-      </c>
-      <c r="E16" s="32"/>
-    </row>
-    <row r="17" spans="3:5" x14ac:dyDescent="0.35">
-      <c r="C17" s="2"/>
-      <c r="D17" s="2"/>
+      <c r="D16" s="29"/>
+      <c r="E16" s="20" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="17" spans="4:5" x14ac:dyDescent="0.35">
       <c r="E17" s="2"/>
     </row>
-    <row r="18" spans="3:5" x14ac:dyDescent="0.35">
-      <c r="C18" s="2"/>
-      <c r="D18" s="2"/>
+    <row r="18" spans="4:5" x14ac:dyDescent="0.35">
       <c r="E18" s="2"/>
     </row>
-    <row r="19" spans="3:5" x14ac:dyDescent="0.35">
-      <c r="C19" s="2"/>
-      <c r="D19" s="2"/>
+    <row r="19" spans="4:5" x14ac:dyDescent="0.35">
       <c r="E19" s="2"/>
     </row>
-    <row r="20" spans="3:5" x14ac:dyDescent="0.35">
-      <c r="C20" s="18"/>
-      <c r="D20" s="18"/>
+    <row r="20" spans="4:5" x14ac:dyDescent="0.35">
       <c r="E20" s="18"/>
     </row>
-    <row r="21" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="21" spans="4:5" x14ac:dyDescent="0.35">
       <c r="D21" s="18"/>
     </row>
   </sheetData>
@@ -998,6 +937,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x0101003C92299DAADCBA47878603B2F45C3285" ma:contentTypeVersion="2" ma:contentTypeDescription="Crie um novo documento." ma:contentTypeScope="" ma:versionID="4fc9d7e97b60d6960c245cc5a329b90f">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="f5932791-1e85-441e-ae00-364d712aba5f" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="d733cda6da82c99407c8fb28615c3c54" ns2:_="">
     <xsd:import namespace="f5932791-1e85-441e-ae00-364d712aba5f"/>
@@ -1129,15 +1077,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -1145,6 +1084,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BFD856F1-1EB0-47D3-9C83-A697C9AFE147}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7A944D73-4D95-470E-B521-C00AAEDFD48B}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1162,14 +1109,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BFD856F1-1EB0-47D3-9C83-A697C9AFE147}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5F18646D-870C-482B-BBB7-0F1BEBF84877}">
   <ds:schemaRefs>

</xml_diff>